<commit_message>
Fixed rendering errors. Included the pertinent variables
</commit_message>
<xml_diff>
--- a/data/form_master.xlsx
+++ b/data/form_master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dflores/Dropbox/EXTS/Projects/autoHiring/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{960D8029-58B5-7244-B077-6627A3974C9B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99AEDBF3-DFE5-474D-A217-686220B7B5CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="460" windowWidth="24540" windowHeight="17540" activeTab="1" xr2:uid="{7A64A84C-17F9-2548-864F-7F5C3007427B}"/>
+    <workbookView xWindow="14300" yWindow="1920" windowWidth="24540" windowHeight="17540" xr2:uid="{7A64A84C-17F9-2548-864F-7F5C3007427B}"/>
   </bookViews>
   <sheets>
     <sheet name="Details" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="100">
   <si>
     <t>First Name</t>
   </si>
@@ -294,6 +294,39 @@
   </si>
   <si>
     <t>Independent/In collaboration</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>Chateau de Signal</t>
+  </si>
+  <si>
+    <t>Blonay</t>
+  </si>
+  <si>
+    <t>JONES</t>
+  </si>
+  <si>
+    <t>MA</t>
+  </si>
+  <si>
+    <t>Music</t>
+  </si>
+  <si>
+    <t>U.K.</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Musician</t>
+  </si>
+  <si>
+    <t>R</t>
   </si>
 </sst>
 </file>
@@ -406,7 +439,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -465,6 +498,9 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -783,8 +819,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42D2E135-155D-3F42-BE22-6B196658E3B7}">
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -821,7 +857,9 @@
       <c r="B5" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="4"/>
+      <c r="C5" s="4" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
@@ -830,7 +868,9 @@
       <c r="B6" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="4"/>
+      <c r="C6" s="4" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
@@ -848,7 +888,9 @@
       <c r="B8" s="17">
         <v>30992</v>
       </c>
-      <c r="C8" s="18"/>
+      <c r="C8" s="18">
+        <v>17175</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
@@ -857,7 +899,9 @@
       <c r="B9" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C9" s="4"/>
+      <c r="C9" s="4" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
@@ -873,7 +917,9 @@
       <c r="B11" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="4"/>
+      <c r="C11" s="4" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
@@ -882,7 +928,9 @@
       <c r="B12" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="C12" s="4"/>
+      <c r="C12" s="4" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
@@ -891,7 +939,9 @@
       <c r="B13" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="C13" s="4"/>
+      <c r="C13" s="4" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
@@ -900,7 +950,9 @@
       <c r="B14" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="C14" s="4"/>
+      <c r="C14" s="4" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
@@ -909,7 +961,9 @@
       <c r="B15" s="5">
         <v>2</v>
       </c>
-      <c r="C15" s="4"/>
+      <c r="C15" s="4">
+        <v>3</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
@@ -918,7 +972,9 @@
       <c r="B16" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="C16" s="4"/>
+      <c r="C16" s="4" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
@@ -936,7 +992,9 @@
       <c r="B18" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="C18" s="4"/>
+      <c r="C18" s="4" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
@@ -945,7 +1003,9 @@
       <c r="B19" s="17">
         <v>38852</v>
       </c>
-      <c r="C19" s="18"/>
+      <c r="C19" s="18">
+        <v>23197</v>
+      </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
@@ -954,7 +1014,9 @@
       <c r="B20" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C20" s="4"/>
+      <c r="C20" s="4" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
@@ -963,7 +1025,9 @@
       <c r="B21" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="C21" s="4"/>
+      <c r="C21" s="4" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
@@ -981,7 +1045,9 @@
       <c r="B23" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="C23" s="4"/>
+      <c r="C23" s="4" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
@@ -990,7 +1056,9 @@
       <c r="B24" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="C24" s="4"/>
+      <c r="C24" s="4" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="13" t="s">
@@ -999,7 +1067,9 @@
       <c r="B25" s="17">
         <v>44105</v>
       </c>
-      <c r="C25" s="18"/>
+      <c r="C25" s="18">
+        <v>42370</v>
+      </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="13" t="s">
@@ -1008,7 +1078,9 @@
       <c r="B26" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C26" s="4"/>
+      <c r="C26" s="4" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="13" t="s">
@@ -1017,7 +1089,9 @@
       <c r="B27" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="C27" s="4"/>
+      <c r="C27" s="4" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="13" t="s">
@@ -1026,7 +1100,9 @@
       <c r="B28" s="16">
         <v>0.8</v>
       </c>
-      <c r="C28" s="4"/>
+      <c r="C28" s="26">
+        <v>1</v>
+      </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="13" t="s">
@@ -1035,7 +1111,9 @@
       <c r="B29" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C29" s="4"/>
+      <c r="C29" s="4" t="s">
+        <v>24</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1046,8 +1124,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C857E2B-D421-6346-9715-70BF747CB052}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -1073,9 +1151,9 @@
       <c r="A3" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="10">
+      <c r="B3" s="10" t="str">
         <f>Details!C5</f>
-        <v>0</v>
+        <v>JONES</v>
       </c>
       <c r="C3" s="7"/>
     </row>
@@ -1083,9 +1161,9 @@
       <c r="A4" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B4" s="10" t="str">
         <f>Details!C6</f>
-        <v>0</v>
+        <v>David</v>
       </c>
       <c r="C4" s="7"/>
     </row>
@@ -1095,7 +1173,7 @@
       </c>
       <c r="B5" s="12">
         <f>Details!C8</f>
-        <v>0</v>
+        <v>17175</v>
       </c>
       <c r="C5" s="7"/>
     </row>
@@ -1103,9 +1181,9 @@
       <c r="A6" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6" s="10" t="str">
         <f>Details!C20</f>
-        <v>0</v>
+        <v>Music</v>
       </c>
       <c r="C6" s="7"/>
     </row>
@@ -1115,7 +1193,7 @@
       </c>
       <c r="B7" s="19">
         <f>Details!C25</f>
-        <v>0</v>
+        <v>42370</v>
       </c>
       <c r="C7" s="7"/>
     </row>
@@ -1141,9 +1219,9 @@
       <c r="A10" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="10">
+      <c r="B10" s="10" t="str">
         <f>Details!C26</f>
-        <v>0</v>
+        <v>Musician</v>
       </c>
       <c r="C10" s="7"/>
     </row>
@@ -1160,7 +1238,7 @@
       </c>
       <c r="B12" s="10">
         <f>Details!C25</f>
-        <v>0</v>
+        <v>42370</v>
       </c>
       <c r="C12" s="7"/>
     </row>
@@ -1186,7 +1264,7 @@
       </c>
       <c r="B15" s="10">
         <f>Details!C28</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15" s="7"/>
     </row>
@@ -1217,7 +1295,7 @@
   <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -1250,7 +1328,7 @@
       </c>
       <c r="B4" s="19">
         <f>Details!C25</f>
-        <v>0</v>
+        <v>42370</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1259,7 +1337,7 @@
       </c>
       <c r="B5" s="11">
         <f>DATE(YEAR(B4) + 1, MONTH(B4), DAY(B4))</f>
-        <v>366</v>
+        <v>42736</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1298,18 +1376,18 @@
       <c r="A10" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="10">
+      <c r="B10" s="10" t="str">
         <f>Details!C5</f>
-        <v>0</v>
+        <v>JONES</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="10">
+      <c r="B11" s="10" t="str">
         <f>Details!C6</f>
-        <v>0</v>
+        <v>David</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -1325,9 +1403,9 @@
       <c r="A13" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="10">
+      <c r="B13" s="10" t="str">
         <f>Details!C9</f>
-        <v>0</v>
+        <v>Chateau de Signal</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -1343,27 +1421,27 @@
       <c r="A15" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="10">
+      <c r="B15" s="10" t="str">
         <f>Details!C11</f>
-        <v>0</v>
+        <v>Blonay</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="10">
+      <c r="B16" s="10" t="str">
         <f>Details!C12</f>
-        <v>0</v>
+        <v>VD</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="10">
+      <c r="B17" s="10" t="str">
         <f>Details!C13</f>
-        <v>0</v>
+        <v>Switzerland</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1372,16 +1450,16 @@
       </c>
       <c r="B18" s="19">
         <f>Details!C8</f>
-        <v>0</v>
+        <v>17175</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="10">
+      <c r="B19" s="10" t="str">
         <f>Details!C14</f>
-        <v>0</v>
+        <v>Married</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -1390,7 +1468,7 @@
       </c>
       <c r="B20" s="10">
         <f>Details!C15</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -1406,27 +1484,27 @@
       <c r="A22" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="10">
+      <c r="B22" s="10" t="str">
         <f>Details!C21</f>
-        <v>0</v>
+        <v>U.K.</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="10">
+      <c r="B23" s="10" t="str">
         <f>Details!C20</f>
-        <v>0</v>
+        <v>Music</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="B24" s="10">
+      <c r="B24" s="10" t="str">
         <f>Details!C16</f>
-        <v>0</v>
+        <v>No</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -1435,7 +1513,7 @@
       </c>
       <c r="B25" s="19">
         <f>Details!C19</f>
-        <v>0</v>
+        <v>23197</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -1453,25 +1531,25 @@
       </c>
       <c r="B27" s="20">
         <f>Details!C28</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B28" s="21">
+      <c r="B28" s="21" t="str">
         <f>Details!C29</f>
-        <v>0</v>
+        <v>Lausanne</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B29" s="10">
+      <c r="B29" s="10" t="str">
         <f>Details!C24</f>
-        <v>0</v>
+        <v>C</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>